<commit_message>
Time sheet updated for 30th jan 2012
</commit_message>
<xml_diff>
--- a/Time_sheet.xlsx
+++ b/Time_sheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="404" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="209" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="15">
   <si>
     <t>Time Sheet for Development of Relational Object Mapping Tool</t>
   </si>
@@ -59,6 +59,9 @@
   </si>
   <si>
     <t>MT2011030</t>
+  </si>
+  <si>
+    <t>Nothing</t>
   </si>
 </sst>
 </file>
@@ -192,20 +195,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="F10" activeCellId="0" pane="topLeft" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.7137254901961"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.2862745098039"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.9882352941176"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.54117647058824"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.6392156862745"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.0901960784314"/>
-    <col collapsed="false" hidden="false" max="257" min="7" style="0" width="8.60392156862745"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.8705882352941"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.4705882352941"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.1411764705882"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.64705882352941"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.8313725490196"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.2392156862745"/>
+    <col collapsed="false" hidden="false" max="257" min="7" style="0" width="8.71372549019608"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="1">
@@ -302,6 +305,66 @@
       </c>
       <c r="F6" s="6" t="n">
         <v>2</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="8">
+      <c r="A8" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="5" t="n">
+        <v>40936</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="9">
+      <c r="A9" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="5" t="n">
+        <v>40936</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="10">
+      <c r="A10" s="6" t="n">
+        <v>3</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="7" t="n">
+        <v>40937</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="6" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -330,7 +393,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="257" min="1" style="0" width="8.60392156862745"/>
+    <col collapsed="false" hidden="false" max="257" min="1" style="0" width="8.71372549019608"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -355,7 +418,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="257" min="1" style="0" width="8.60392156862745"/>
+    <col collapsed="false" hidden="false" max="257" min="1" style="0" width="8.71372549019608"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>